<commit_message>
sync copysheet from xssf examples
</commit_message>
<xml_diff>
--- a/examples/xssf/CopySheet/file1.xlsx
+++ b/examples/xssf/CopySheet/file1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WIP\Legacy\NPOI\npoi-core-0.1\examples\xssf\CopySheet\oldFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\npoi\examples\xssf\CopySheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210B0CE8-B904-4138-8F87-22D6859A0304}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F99BD08-EF30-4080-A3DD-D604F683A341}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{462009CC-69BC-4117-AA6B-053E13E8DE35}"/>
+    <workbookView xWindow="3270" yWindow="2205" windowWidth="23025" windowHeight="13395" xr2:uid="{462009CC-69BC-4117-AA6B-053E13E8DE35}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,11 +60,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -74,8 +74,15 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -104,7 +111,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -120,7 +127,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -419,12 +426,12 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,12 +445,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -451,12 +458,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>